<commit_message>
miscellaneous bug fixes and prompt engineering
</commit_message>
<xml_diff>
--- a/src/evaluation/model_answers.xlsx
+++ b/src/evaluation/model_answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[{"nugget": "The condenser has a single failure mode: leaking.", "status": "ESSENTIAL"}, {"nugget": "The RPN for the leaking failure mode of the condenser is 18.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The condenser has a single failure mode: leaking.", "status": "ESSENTIAL"}, {"nugget": "The RPN (Risk Priority Number) for the condenser's leaking failure mode is 18.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[{"nugget": "The subsystem for the Engine is Power Unit.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The subsystem for the engine is Power Unit.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[{"nugget": "The failure mode in question is Wearing on the Transmission Mount.", "status": "ESSENTIAL"}, {"nugget": "The recommended action is to check bolt connection torques.", "status": "ESSENTIAL"}, {"nugget": "The bolt connection torques should be checked at the 500 hour service interval.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The failure mode is wearing on the transmission mount sub-component.", "status": "ESSENTIAL"}, {"nugget": "The recommended action is to check bolt connection torques.", "status": "ESSENTIAL"}, {"nugget": "The action should be carried out at 500 hour service intervals.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[{"nugget": "The subcomponent 'Fuses' of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The subcomponent 'Wiring Harness' of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The subcomponent 'Turbocharger' of the Power Unit has an RPN of 27.", "status": "OPTIONAL"}]</t>
+          <t>[{"nugget": "The subcomponent Fuses in the component Electrical System of the Power Unit has an RPN of 27 for the failure mode Overloading.", "status": "ESSENTIAL"}, {"nugget": "The subcomponent Wiring Harness in the component Electrical System of the Power Unit has an RPN of 27 for the failure mode Corrosion.", "status": "ESSENTIAL"}, {"nugget": "The subcomponent Turbocharger in the component Air Intake System of the Power Unit has an RPN of 27 for the failure mode Mechanical Failure.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[{"nugget": "The failure mode in the air intake system with a recommended action is 'Reaches end of usable life.'", "status": "ESSENTIAL"}, {"nugget": "This failure mode occurs in the air filter subcomponent.", "status": "ESSENTIAL"}, {"nugget": "The recommended action is to check air filter indicators during daily inspections.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The Air Intake System has a failure mode with a recommended action.", "status": "ESSENTIAL"}, {"nugget": "The failure mode is 'Reaches end of usable life'.", "status": "ESSENTIAL"}, {"nugget": "The failure mode occurs in the Air filter subcomponent.", "status": "ESSENTIAL"}, {"nugget": "The recommended action is to check air filter indicators during daily inspections.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[{"nugget": "The cause of ECU overloading in the power train can be shorting of a sensor power surge.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The cause of ECU overload in the power train can be shorting due to a sensor power surge.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[{"nugget": "The Power Unit is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Power Train is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Hydraulic System is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Electrical System is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Power Frame is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Load Frame is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}, {"nugget": "The Fire Suppression System is a subsystem available in the knowledge base.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The knowledge base includes a Power Unit subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes a Power Train subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes a Hydraulic System subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes an Electrical System subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes a Power Frame subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes a Load Frame subsystem.", "status": "ESSENTIAL"}, {"nugget": "The knowledge base includes a Fire Suppression System subsystem.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[{"nugget": "An air conditioner contains a compressor as a main component.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a condenser as a main component.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains an evaporator as a main component.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a fan as a main component.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a filter as a main component.", "status": "OPTIONAL"}, {"nugget": "An air conditioner contains a filter housing as a main component.", "status": "OPTIONAL"}, {"nugget": "An air conditioner contains vents as a main component.", "status": "OPTIONAL"}]</t>
+          <t>[{"nugget": "An air conditioner contains a compressor.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a condenser.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains an evaporator.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a fan.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains a filter.", "status": "ESSENTIAL"}, {"nugget": "An air conditioner contains filter housing.", "status": "OPTIONAL"}, {"nugget": "An air conditioner contains vents.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[{"nugget": "The failure mode 'Corrosion' for Batteries has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "The failure mode 'Wearing' for Batteries has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "The failure mode 'End of usable life' for Batteries has an RPN of 12.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Corrosion is a failure mode of the Batteries subcomponent with an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Wearing is a failure mode of the Batteries subcomponent with an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "End of usable life is a failure mode of the Batteries subcomponent with an RPN of 12.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[{"nugget": "Transmission in the Power Train subsystem contains failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Electronic control unit (ECU) of the Transmission has an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Electronic control unit (ECU) of the Transmission has an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Planetary Gear Sets of the Transmission has an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "Upbox in the Power Train subsystem contains failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Gears of the Upbox has an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "Dropbox in the Power Train subsystem contains failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Gears of the Dropbox has an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "Cooling System in the Power Unit subsystem contains failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Mechanical Failure in the Water Pump of the Cooling System has an RPN of 36.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Transmission in the Power Train subsystem has at least one failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Upbox in the Power Train subsystem has at least one failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Dropbox in the Power Train subsystem has at least one failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Cooling System in the Power Unit subsystem has at least one failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the ECU subcomponent of the Transmission has an RPN of 36.", "status": "OPTIONAL"}, {"nugget": "Corrosion in the ECU subcomponent of the Transmission has an RPN of 36.", "status": "OPTIONAL"}, {"nugget": "Wearing in the Planetary Gear Sets subcomponent of the Transmission has an RPN of 36.", "status": "OPTIONAL"}, {"nugget": "Wearing in the Gears subcomponent of the Upbox has an RPN of 36.", "status": "OPTIONAL"}, {"nugget": "Wearing in the Gears subcomponent of the Dropbox has an RPN of 36.", "status": "OPTIONAL"}, {"nugget": "Mechanical Failure in the Water Pump subcomponent of the Cooling System has an RPN of 36.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[{"nugget": "No component has a failure mode with an RPN value over 40.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "No components have failure modes with an RPN value over 40.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[{"nugget": "Fuel Filter subcomponent in the Fuel System of the Power Unit subsystem has the Blocked failure mode.", "status": "ESSENTIAL"}, {"nugget": "Oil Cooler subcomponent in the Lubrication System of the Power Unit subsystem has the Blocked failure mode.", "status": "ESSENTIAL"}, {"nugget": "Oil Filter subcomponent in the Lubrication System of the Power Unit subsystem has the Blocked failure mode.", "status": "ESSENTIAL"}, {"nugget": "Lubrication lines subcomponent in the Lubrication System of the Power Unit subsystem has the Blocked failure mode.", "status": "ESSENTIAL"}, {"nugget": "Filter subcomponent in the Air-conditioning of the Electrical System subsystem has the Blocked failure mode.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Fuel Filter in the Fuel System (Power Unit subsystem) has the failure mode Blocked.", "status": "ESSENTIAL"}, {"nugget": "Oil Cooler in the Lubrication System (Power Unit subsystem) has the failure mode Blocked.", "status": "ESSENTIAL"}, {"nugget": "Oil Filter in the Lubrication System (Power Unit subsystem) has the failure mode Blocked.", "status": "ESSENTIAL"}, {"nugget": "Lubrication lines in the Lubrication System (Power Unit subsystem) have the failure mode Blocked.", "status": "ESSENTIAL"}, {"nugget": "Filter in the Air-conditioning (Electrical System subsystem) has the failure mode Blocked.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[{"nugget": "The Power Unit subsystem has several failure modes associated with leaks (e.g., Cracked or leaking, Leaking, Leak or Leaks).", "status": "ESSENTIAL"}, {"nugget": "The Cooling System component in the Power Unit subsystem has the failure mode 'Leaks' with the highest occurrence value for leak-related failures.", "status": "ESSENTIAL"}, {"nugget": "The Radiator is a subcomponent of the Cooling System component where this occurs.", "status": "ESSENTIAL"}, {"nugget": "The highest occurrence value for these leak-related failure modes is 4.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "There are several failure modes associated with leaks in the Power Unit subsystem: Cracked or leaking, Leaking, Leak or Leaks.", "status": "OPTIONAL"}, {"nugget": "The failure mode with the highest occurrence value for leaks in the Power Unit subsystem is 'Leaks' in the Cooling System component.", "status": "ESSENTIAL"}, {"nugget": "The 'Leaks' failure mode with the highest occurrence is specifically in the Radiator subcomponent of the Cooling System.", "status": "ESSENTIAL"}, {"nugget": "The occurrence value for this failure mode is 4.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[{"nugget": "The most detectable failure mode in the Power Train subsystem is Wearing.", "status": "ESSENTIAL"}, {"nugget": "This failure mode has a detection value of 5.", "status": "ESSENTIAL"}, {"nugget": "The Wearing failure mode occurs in the Axles component.", "status": "ESSENTIAL"}, {"nugget": "The Wearing failure mode is associated with the Differential subcomponent.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The failure mode with the highest detection value in the Power Train subsystem is Wearing.", "status": "ESSENTIAL"}, {"nugget": "This failure mode occurs in the Axles component.", "status": "ESSENTIAL"}, {"nugget": "This failure mode occurs in the Differential subcomponent.", "status": "ESSENTIAL"}, {"nugget": "The detection value for this failure mode is 5.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>How many distinct sub-components are listed in the data</t>
+          <t>How many sub-components are listed in the data</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[{"nugget": "There are 167 sub-components listed in the data.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "There are 167 sub-components in the data (knowledge base).", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[{"nugget": "The average RPN of all failure modes for the Charging and Ignition component is 20.", "status": "ESSENTIAL"}, {"nugget": "There are 14 different failure modes considered for the Charging and Ignition component.", "status": "OPTIONAL"}]</t>
+          <t>[{"nugget": "The average RPN of all failure modes for the charging and ignition component of the electrical system is 20.", "status": "ESSENTIAL"}, {"nugget": "There are 14 different failure modes for the charging and ignition component of the electrical system.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -882,7 +882,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[{"nugget": "There are two entities named 'Electrical System': one as a subsystem and one as a component of the Power Unit subsystem.", "status": "ESSENTIAL"}, {"nugget": "Only the Electrical System component of the Power Unit subsystem has failure modes that result in fire as a possible failure effect.", "status": "ESSENTIAL"}, {"nugget": "The most likely failure modes causing fire have an occurrence value of 3.", "status": "ESSENTIAL"}, {"nugget": "One likely failure mode is shorting of connections or incorrect rating of fuse installed, leading to fire, with loss of function and engine shutdown.", "status": "ESSENTIAL"}, {"nugget": "Another likely failure mode is exposure to contaminants over time causing ineffective terminal connections and brittle wires, leading to fire, with loss of function and engine shutdown.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "There are two entities named Electrical System: one is a subsystem and one is a component of the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "Only the component electrical system has failure modes with fire as a possible failure effect.", "status": "ESSENTIAL"}, {"nugget": "The most likely failure modes with fire have an occurrence value of 3.", "status": "ESSENTIAL"}, {"nugget": "One likely failure cause is shorting of connections due to incorrect rating of fuse installed, leading to loss of function, fire, and engine shutdown.", "status": "ESSENTIAL"}, {"nugget": "Another likely failure cause is terminal connections being ineffective and wires becoming brittle due to exposure to contaminants over time, leading to loss of function, fire, and engine shutdown.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[{"nugget": "The component with the highest number of failures is the Data Collection Unit (DCU).", "status": "ESSENTIAL"}, {"nugget": "The DCU is part of the Electrical System subsystem.", "status": "ESSENTIAL"}, {"nugget": "The DCU has 41 failure modes.", "status": "ESSENTIAL"}, {"nugget": "All failure modes of the DCU have a severity of 2.", "status": "ESSENTIAL"}, {"nugget": "There is no single most severe failure mode for the DCU because all modes have the same severity.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The component with the highest number of failures is the Data Collection Unit (DCU).", "status": "ESSENTIAL"}, {"nugget": "The DCU is part of the Electrical System subsystem.", "status": "OPTIONAL"}, {"nugget": "The DCU has 41 failure modes.", "status": "ESSENTIAL"}, {"nugget": "There is no single most severe failure mode for the DCU; all its failure modes have a severity of 2.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[{"nugget": "There are failure modes with RPN greater than or equal to 25, detection rating of 2 or less, and no recommended action.", "status": "ESSENTIAL"}, {"nugget": "One such failure mode is Mechanical Failure in the Power Unit subsystem, Engine component, Belts subcomponent.", "status": "ESSENTIAL"}, {"nugget": "This Mechanical Failure has an RPN of 32 and a detection rating of 2.", "status": "ESSENTIAL"}, {"nugget": "There is another failure mode: Out of date / no test tag in the Fire Suppression System subsystem, AFFF component, Activation System &amp; Gauge subcomponent.", "status": "ESSENTIAL"}, {"nugget": "This Out of date / no test tag failure mode has an RPN of 32 and detection of 2.", "status": "ESSENTIAL"}, {"nugget": "Neither failure mode currently has a recommended action.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Mechanical Failure in the Power Unit subsystem, Engine component, Belts subcomponent, is a failure mode with an RPN of 32, detection rating of 2, and no recommended action.", "status": "ESSENTIAL"}, {"nugget": "Out of date / no test tag in the Fire Suppression System subsystem, AFFF component, Activation System &amp; Gauge subcomponent, is a failure mode with an RPN of 32, detection rating of 2, and no recommended action.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[{"nugget": "43% of hydraulic system failure modes have an RPN above 15.", "status": "ESSENTIAL"}, {"nugget": "12 out of 28 failure modes have an RPN above 15.", "status": "OPTIONAL"}]</t>
+          <t>[{"nugget": "43% of hydraulic system failure modes have an RPN above 15.", "status": "ESSENTIAL"}, {"nugget": "12 out of 28 hydraulic system failure modes have an RPN above 15.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[{"nugget": "Cracked or Leaking in the Power Unit subsystem, Fuel System component, and Fuel Tank subcomponent has multiple causes: General wear and tear and Physical impact to tank.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Power Train subsystem, Axles component, and Differential subcomponent has multiple causes: Servicing error, Blocking of breather cap, poor storage or mixing of oils, and servicing error.", "status": "ESSENTIAL"}, {"nugget": "Loose fittings in the Power Train subsystem, Drivelines component, and Articulation Driveline subcomponent has multiple causes: Vibration causing loose bolts and universal joints, and Wearing of articulation bearings over time.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Cracked or Leaking failure mode in the Fuel Tank subcomponent of the Fuel System component, within the Power Unit subsystem, has multiple causes: General wear and tear, and Physical impact to tank.", "status": "ESSENTIAL"}, {"nugget": "Wearing failure mode in the Differential subcomponent of the Axles component, within the Power Train subsystem, has multiple causes: Servicing error, Blocking of breather cap, poor storage or mixing of oils, and servicing error.", "status": "ESSENTIAL"}, {"nugget": "Loose fittings failure mode in the Articulation Driveline subcomponent of the Drivelines component, within the Power Train subsystem, has multiple causes: Vibration causing loose bolts and universal joints, and Wearing of articulation bearings over time.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[{"nugget": "The Fittings subcomponent in the Hydraulic System subsystem does not have a failure mode called Blockage.", "status": "ESSENTIAL"}, {"nugget": "The Valves component in the Hydraulic System subsystem does not have a failure mode called Blockage.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The Fittings subcomponent in the Hydraulic System does not have a failure mode called Blockage.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[{"nugget": "The fan drive assembly in the power unit has a single failure mode: wearing.", "status": "ESSENTIAL"}, {"nugget": "The cause of this wearing failure mode is wearing over time.", "status": "ESSENTIAL"}, {"nugget": "Wearing of the fan drive assembly may lead to heating of the power unit as a failure effect.", "status": "ESSENTIAL"}, {"nugget": "Overheating is an effect, not a cause, of wearing in the fan drive assembly.", "status": "ESSENTIAL"}, {"nugget": "Physical impact is not identified as a cause of wearing in the fan drive assembly.", "status": "ESSENTIAL"}, {"nugget": "The more likely cause of wearing is wearing over time, not physical impact or overheating.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "The fan drive assembly in the power unit has a single failure mode called 'Wearing'.", "status": "ESSENTIAL"}, {"nugget": "The failure cause for 'Wearing' is wearing over time.", "status": "ESSENTIAL"}, {"nugget": "Wearing is not primarily caused by physical impact or overheating.", "status": "ESSENTIAL"}, {"nugget": "Wearing of the fan drive assembly could result in heating of the power unit as a failure effect.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[{"nugget": "There are no recommended actions for corrosion of the wiper motor under Cabin Controls.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "No actions have been recommended for the corrosion failure mode on the wiper motor of the cabin controls.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[{"nugget": "Cracked or leaking in the Fuel Tank can cause fuel loss and fire.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Fuel Cooler can cause loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Fuel Cooler can cause loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Mechanical failure in the Fuel Cooler can cause fuel overheating.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Filter can cause loss of power and fire.", "status": "OPTIONAL"}, {"nugget": "Physical damage in the Fuel Filter can cause fuel leak and fire.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Fuel Lines/Rail can cause loss of power and fire.", "status": "OPTIONAL"}, {"nugget": "Physical damage in the Fuel Lines/Rail can cause loss of power and fire.", "status": "OPTIONAL"}]</t>
+          <t>[{"nugget": "Cracked or leaking in the Fuel Tank can lead to effects such as fuel loss and fire.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Cooler can cause loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Fuel Cooler can result in loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Mechanical failure in the Fuel Cooler can cause fuel overheating.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Filter can lead to loss of power and fire.", "status": "OPTIONAL"}, {"nugget": "Physical damage in the Fuel Filter can result in fuel leak and fire.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Fuel Lines/Rail can lead to loss of power and fire.", "status": "OPTIONAL"}, {"nugget": "Physical damage in the Fuel Lines/Rail can result in loss of power and fire.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[{"nugget": "List all subsystems in descending order based on their average occurrence values.", "status": "ESSENTIAL"}, {"nugget": "The Load Frame subsystem has an average occurrence value of 3.0.", "status": "ESSENTIAL"}, {"nugget": "The Fire Suppression System subsystem has an average occurrence value of 2.615.", "status": "ESSENTIAL"}, {"nugget": "The Power Train subsystem has an average occurrence value of 2.529.", "status": "ESSENTIAL"}, {"nugget": "The Hydraulic System subsystem has an average occurrence value of 2.464.", "status": "ESSENTIAL"}, {"nugget": "The Power Frame subsystem has an average occurrence value of 2.45.", "status": "ESSENTIAL"}, {"nugget": "The Power Unit subsystem has an average occurrence value of 2.301.", "status": "ESSENTIAL"}, {"nugget": "The Electrical System subsystem has an average occurrence value of 2.197.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "List the subsystems in descending order of their average occurrence values.", "status": "ESSENTIAL"}, {"nugget": "Load Frame has an average occurrence value of 3.0.", "status": "ESSENTIAL"}, {"nugget": "Fire Suppression System has an average occurrence value of 2.615.", "status": "ESSENTIAL"}, {"nugget": "Power Train has an average occurrence value of 2.529.", "status": "ESSENTIAL"}, {"nugget": "Hydraulic System has an average occurrence value of 2.464.", "status": "ESSENTIAL"}, {"nugget": "Power Frame has an average occurrence value of 2.45.", "status": "ESSENTIAL"}, {"nugget": "Power Unit has an average occurrence value of 2.301.", "status": "ESSENTIAL"}, {"nugget": "Electrical System has an average occurrence value of 2.197.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
@@ -1128,45 +1128,289 @@
 • Leaking in the Suspension Cylinder subcomponent, with the failure cause General wear and tear, Physical impacts, incorrect installation of seals
 • Wearing in the Suspension Bushing subcomponent, with the failure cause Wearing over time
 • Leaking in the Steering Cylinder subcomponent, with the failure cause General wear and tear, steering controll valve failure, incorrect installation of seals
-• Leaking in the Hoist Cylinder subcompoennt, with the failure cause General wear and tear, physical impacts, incorrect installation of seal or cylinder
+• Leaking in the Hoist Cylinder subcomponent, with the failure cause General wear and tear, physical impacts, incorrect installation of seal or cylinder
 </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[{"nugget": "Leaking in the Suspension Cylinder can occur due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Suspension Cylinder can occur due to physical impacts.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Suspension Cylinder can occur due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Suspension Bushing can occur due to wearing over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Steering Cylinder can occur due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Steering Cylinder can occur due to steering controll valve failure.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Steering Cylinder can occur due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Hoist Cylinder can occur due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Hoist Cylinder can occur due to physical impacts.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Hoist Cylinder can occur due to incorrect installation of seals or cylinder.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "Leaking can occur in the Suspension Cylinder subcomponent due to general wear and tear over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Suspension Cylinder subcomponent due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Wearing can occur in the Suspension Bushing subcomponent due to wear over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Steering Cylinder subcomponent due to general wear and tear over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Steering Cylinder subcomponent due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Hoist Cylinder subcomponent due to general wear and tear over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Hoist Cylinder subcomponent due to incorrect installation of seals or cylinder components.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Suspension Cylinder can be caused by physical impacts.", "status": "OPTIONAL"}, {"nugget": "Leaking in the Hoist Cylinder can be caused by physical impacts.", "status": "OPTIONAL"}]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Give me some information and summary statistics about the hydraulic system.</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
+          <t>Are there any recommended actions that prescribe actions past just a check in the fuel system?</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">There is one recommended action above simple checking - Drain and flush fuel tank during 1000 hour service. on the Cracked and leaking failure mode. This is located in the Fuel Tank subcomponent of the Fuel System component.
+</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>[{"nugget": "No information about the hydraulic system was provided in the answer.", "status": "ESSENTIAL"}]</t>
+          <t>[{"nugget": "There is one recommended action beyond just checking in the fuel system.", "status": "ESSENTIAL"}, {"nugget": "The action is to drain and flush the fuel tank during 1000 hour service.", "status": "ESSENTIAL"}, {"nugget": "This action is prescribed for the 'Cracked and leaking' failure mode.", "status": "ESSENTIAL"}, {"nugget": "The failure mode and action pertain to the Fuel Tank subcomponent of the Fuel System component.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>How many failure modes are there for the Upbox Housing?</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">There is only one failure mode for the Housing subcomponent of the Upbox component, called Wearing.
+</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>[{"nugget": "The Upbox Housing subcomponent has only one failure mode.", "status": "ESSENTIAL"}, {"nugget": "The failure mode for the Housing is called Wearing.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What current controls on the Air Intake System are just to perform a check on a regular interval. 
+</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Air Intake System Component has the following current controls that simply involve performing a regular check:
+• Visual inspection daily for damages for the Physical Damage failure mode on the Air filter housing subcomponent.
+• Inspect induction hoses and joints every 125 hour service for the Leaking failure mode on the Turbocharger subcomponent.
+• Visual inspection on 125 hour services for the Physical damage failure mode on the Charge Air Cooler subcomponent.
+• Visual inspection on 125 hour services for the Physical damage failure mode on the Inlet Manifold subcomponent.
+• Visual inspection on 125 hour services for the Leaking failure mode on the Inlet Manifold subcomponent.
+</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Perform a daily visual inspection for damages to the Air filter housing to check for Physical Damage failure mode.", "status": "ESSENTIAL"}, {"nugget": "Inspect induction hoses and joints every 125 hour service on the Turbocharger to check for Leaking failure mode.", "status": "ESSENTIAL"}, {"nugget": "Perform a visual inspection every 125 hour service on the Charge Air Cooler to check for Physical Damage failure mode.", "status": "ESSENTIAL"}, {"nugget": "Perform a visual inspection every 125 hour service on the Inlet Manifold to check for Physical Damage failure mode.", "status": "ESSENTIAL"}, {"nugget": "Perform a visual inspection every 125 hour service on the Inlet Manifold to check for Leaking failure mode.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>How many failure modes are there for the Upbox Housing?</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>[{"nugget": "No answer about the number of failure modes for the Upbox Housing is provided.", "status": "ESSENTIAL"}]</t>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are there any failure modes affecting personnel safety that do not have a severity score of 3 or above?
+</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some failure modes all with a severity score of 2 that directly affect personnel safety are:
+• Corrosion on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) have the failure effect Reduced ability to successfully move machinery safely.
+• Wearing on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) has the failure effect Reduced ability to successfully move machinery safely.
+• Wearing on the Hand Rails subcomponent of the Power Frame subsystem and Hoods and Covers component has the failure effect Difficulty in gaining access to machine above safe working height.
+• Wearing on the Cabin Assembly subcomponent of the Power Frame subsystem and Cabin component has the failure effect Unsafe Working environment, windows, and doors no longer fit.
+• Wearing on the Drivers Seat subcomponent of the Power Frame subsystem and Cabin component has the failure effect Unsafe working environment. 
+• Wearing on the Windows subcomponent of the Power Frame subsystem and Cabin component has the failure effect Unsafe working environment. 
+• Overloading on the Grease Pump subcomponent of the Power Frame subsystem and Greasing system component has the failure effect Shorting of live wires to ground, or electrical component failure.
+There are also several other failure modes below a severity score of 3 with effects that may indirectly affect personnel safety, such as fire hazards and false readings. 
+</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>[{"nugget": "There exist failure modes affecting personnel safety that have a severity score below 3.", "status": "ESSENTIAL"}, {"nugget": "Some of these failure modes have a severity score of 2 and directly affect personnel safety.", "status": "ESSENTIAL"}, {"nugget": "Corrosion on the Cameras subcomponent (Electrical System subsystem, DCU) causes reduced ability to move machinery safely.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cameras subcomponent (Electrical System subsystem, DCU) causes reduced ability to move machinery safely.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Hand Rails (Power Frame subsystem, Hoods and Covers) causes difficulty in gaining access to machine above safe working height.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cabin Assembly (Power Frame subsystem, Cabin component) causes unsafe working environment due to windows and doors no longer fitting.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Drivers Seat (Power Frame subsystem, Cabin component) causes unsafe working environment.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Windows (Power Frame subsystem, Cabin component) causes unsafe working environment.", "status": "ESSENTIAL"}, {"nugget": "Overloading on the Grease Pump (Power Frame subsystem, Greasing system) causes shorting of live wires to ground or electrical component failure.", "status": "ESSENTIAL"}, {"nugget": "There are other failure modes below a severity score of 3 that may indirectly affect personnel safety, such as fire hazards and false readings.", "status": "OPTIONAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the failure modes in the Power Train subsystem, which have recommended actions related to lubrication?
+</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Power Train subsystem has the following failure modes with recommended actions related to lubrication:
+• Corrosion in the Transmission component and Electronic control unit (ECU) subcomponent, with the recommended action Investigate method to include auto-electrical servicing in PM services. Grease (add sealant) all connections and plugs every 500 hour service.
+• Wearing in the Drivelines component and Articulation Driveline subcompoennt, with the recommended action Inspect and lubricate driveline slip joint and universal joints on 125\ hour service. Inspect for optimal replacement interval of component.
+</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Corrosion failure mode occurs in the Transmission component and ECU subcomponent of the Power Train subsystem.", "status": "ESSENTIAL"}, {"nugget": "Recommended action for corrosion in Transmission/ECU includes greasing (adding sealant) to all connections and plugs every 500 hours.", "status": "ESSENTIAL"}, {"nugget": "Wearing failure mode occurs in the Drivelines component and Articulation Driveline subcomponent of the Power Train subsystem.", "status": "ESSENTIAL"}, {"nugget": "Recommended action for wearing in Drivelines/Articulation Driveline includes inspecting and lubricating the driveline slip joint and universal joints every 125 hours.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>What Failure Modes in the Fuel System are related to overheating?</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Fuel System component has the following failure modes with failure effects related to overheating and high temperatures:
+• Cracked or Leaking in the Fuel Tank subcomponent, with the failure effect Fuel loss, fire.
+• Leaking in the Fuel Cooler subcomponent, with the failure effect Loss of power, engine overheating.
+• Wearing in the Fuel Cooler subcomponent, with the failure effect Loss of power, engine overheating.
+• Mechanical failure in the Fuel Cooler subcomponent, with the failure effect Fuel overheating.
+• Leaking in the Fuel Filter subcomponent, with the failure effect Loss of power, fire.
+• Physical Damage in the Fuel Filter subcomponent, with the failure effect Fuel leak, fire.
+• Leaking in the Fuel Lines/Rail subcomponent, with the failure effect Loss of power, fire.
+• Physical Damage in the Fuel Lines/Rail subcomponent, with the failure effect Loss of power, fire.
+</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Cracks or leaks in the Fuel Tank can cause fuel loss and fire, relating to overheating effects.", "status": "ESSENTIAL"}, {"nugget": "Leaks in the Fuel Cooler can cause loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Wear in the Fuel Cooler can result in loss of power and engine overheating.", "status": "ESSENTIAL"}, {"nugget": "Mechanical failure of the Fuel Cooler can lead to fuel overheating.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">List all the failure modes in the Electrical System's PLC in descending order of their RPN.
+</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The knowledge base has the following 23 failure modes in the Electrical System subsystem and Programmable Logic Controller (PLC) component, in descending order of RPN values:
+1. Corrosion in the Monitor dump box position subcomponent, with an RPN of 27.
+2. The following 5 failure modes, with an RPN of 18:
+    • Overloading in the Monitor dump box position subcomponent.
+    • Corrosion in the Release or set the parking brake subcomponent.
+    • Overloading in the Release or set the parking brake subcomponent.
+    • Corrosion in the Park Brake Switch subcomponent.
+    • Overloading in the Park Brake Switch subcomponent.
+7. The following 12 failure modes, with an RPN of 12:
+    • Wearing in the Monitor dump box position subcomponent.
+    • Corrosion in the Alarms and lights subcomponent.
+    • Wearing in the Alarms and lights subcomponent.
+    • Corrosion in the Reverse Alarm subcomponent.
+    • Wearing in the Reverse Alarm subcomponent.
+    • Physical damage in the Park Brake Switch subcomponent.
+    • Corrosion in the Dash subcomponent.
+    • Overloading in the Dash subcomponent.
+    • Corrosion in the Gears Sensor subcomponent.
+    • Overloading in the Gears Sensor subcomponent.
+    • Corrosion in the Transmission Sensor subcomponent.
+    • Overloading in the Transmission Sensor subcomponent.
+19. The following 5 failure modes, with an RPN of 8:
+    • Overloading in the Alarms and lights subcomponent.
+    • Overloading in the Reverse Alarm subcomponent.
+    • Physical damage in the Dash subcomponent.
+    • Physical damage in the Gears Sensor subcomponent.
+    • Physical damage in the Transmission Sensor subcomponent.
+</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Failure modes in the Electrical System's PLC are listed in descending order of their RPN.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Monitor dump box position subcomponent has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Monitor dump box position subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Release or set the parking brake subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Release or set the parking brake subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Park Brake Switch subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Park Brake Switch subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Monitor dump box position subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Alarms and lights subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Alarms and lights subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Reverse Alarm subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Reverse Alarm subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Park Brake Switch subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Dash subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Dash subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Gears Sensor subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Gears Sensor subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Corrosion in the Transmission Sensor subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Transmission Sensor subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Alarms and lights subcomponent has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "Overloading in the Reverse Alarm subcomponent has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Dash subcomponent has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Gears Sensor subcomponent has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Transmission Sensor subcomponent has an RPN of 8.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Any failure modes with an RPN less than 5? What are their other numerical values?</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The following failure modes have an RPN less than 5:
+• Corrosion in the Electrical System subsystem, Transmission Electronic Control Unit (ECU) component and Solenoid Wiring subcomponent with an RPN of 0. It has a severity of 2, occurrence of 2 and detection of 3. 
+• Wearing in the Power Frame subsystem, Hoods and Covers component and Covers subcomponent with an RPN of 2. It has a severity of 1, occurrence of 2 and detection of 1.
+• Broken in the Power Unit subsystem, Lubrication System component and Dipstick subcomponent with an RPN of 3. It has a severity of 1, occurrence of 3 and detection of 1.
+• Leaking in the Hydraulic System subsystem, Cylinders component and Hoist Cylinder subcomponent with an RPN of 4. It has a severity of 2, occurrence of 1 and detection of 2.
+• Physical damage in the Electrical System subsystem, Data Collection Unit (DCU) component and Gauges subcomponent with an RPN of 4. It has a severity of 2, occurrence of 2 and detection of 1.
+</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Corrosion in the Electrical System subsystem, Transmission Electronic Control Unit (ECU) component, Solenoid Wiring subcomponent has an RPN of 0.", "status": "ESSENTIAL"}, {"nugget": "Corrosion has severity 2, occurrence 2, detection 3.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Power Frame subsystem, Hoods and Covers component, Covers subcomponent has an RPN of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing has severity 1, occurrence 2, detection 1.", "status": "ESSENTIAL"}, {"nugget": "Broken in the Power Unit subsystem, Lubrication System component, Dipstick subcomponent has an RPN of 3.", "status": "ESSENTIAL"}, {"nugget": "Broken has severity 1, occurrence 3, detection 1.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Hydraulic System subsystem, Cylinders component, Hoist Cylinder subcomponent has an RPN of 4.", "status": "ESSENTIAL"}, {"nugget": "Leaking has severity 2, occurrence 1, detection 2.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Electrical System subsystem, Data Collection Unit (DCU) component, Gauges subcomponent has an RPN of 4.", "status": "ESSENTIAL"}, {"nugget": "Physical damage has severity 2, occurrence 2, detection 1.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>What are the failure modes in the Cylinders component of the Hydraulic System, that may be caused by wearing?</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Cylinders component in the Hydraulic System subsystem has the following failure modes with failure causes related to natural degradation over time:
+• Leaking in the Suspension Cylinder subcomponent, with the failure cause General wear and tear, Physical impacts, incorrect installation of seals
+• Wearing in the Suspension Bushing subcomponent, with the failure cause Wearing over time
+• Leaking in the Steering Cylinder subcomponent, with the failure cause General wear and tear, steering controll valve failure, incorrect installation of seals
+• Leaking in the Hoist Cylinder subcomponent, with the failure cause General wear and tear, physical impacts, incorrect installation of seal or cylinder
+</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Leaking can occur in the Suspension Cylinder due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Suspension Cylinder due to physical impacts.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Suspension Cylinder due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Wearing can occur in the Suspension Bushing due to wearing over time.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Steering Cylinder due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Steering Cylinder due to steering control valve failure.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Steering Cylinder due to incorrect installation of seals.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Hoist Cylinder due to general wear and tear.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Hoist Cylinder due to physical impacts.", "status": "ESSENTIAL"}, {"nugget": "Leaking can occur in the Hoist Cylinder due to incorrect installation of seal or cylinder.", "status": "ESSENTIAL"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>What is the potential cause of discharge on the AFFF?</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Unintentional discharge failure mode in the Cylinder subcomponent, of the AFFF component of the Fire Suppression System subsystem, has the failure cause Activation due to line failure or other accidental means.
+The following failure modes also lead to potential failure modes that reference unintentional discharge, so they may be the causes:
+• Wearing in the Hoses subcomponent leads to the potential failure effect Reduced capacity to use effectively, may cause unintentional discharge of AFFF system.
+• Wearing in the Mounting Point subcomponent leads to the potential failure effect May cause damage to the cylinder, loss of cylinder, unintentional discharge of AFFF system.
+• Wearing in the Activation System &amp; Gauge subcomponent leads to the potential failure effect May cause unintentional discharge of AFFF system or inability to discharge system, system pressure may not be accurately displayed.
+</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>[{"nugget": "Unintentional discharge in the AFFF can be caused by activation due to line failure or other accidental means in the Cylinder subcomponent.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Hoses subcomponent can cause unintentional discharge of the AFFF system by reducing the capacity to use effectively.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Mounting Point subcomponent can cause unintentional discharge of the AFFF system by damaging or causing loss of the cylinder.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Activation System &amp; Gauge subcomponent can cause unintentional discharge of the AFFF system, or inability to discharge, or inaccurate system pressure display.", "status": "ESSENTIAL"}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
manual scoring metric calculation + evaluation loop + fuzzy match fixes + misc prompt tweaks
</commit_message>
<xml_diff>
--- a/src/evaluation/model_answers.xlsx
+++ b/src/evaluation/model_answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sellsol/Documents/University/2025 units/Honours project/Code/Hons25_Heidi/src/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14492AD1-755B-7042-B009-0B3031A957B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F634B281-D3D2-0C4E-B958-725AD9044B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1320" windowWidth="26560" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="1480" windowWidth="21120" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Name matching</t>
   </si>
   <si>
-    <t>[{"nugget": "The condenser has a single failure mode: Leaking.", "status": "ESSENTIAL"}, {"nugget": "The RPN for the condenser leaking failure mode is 18.", "status": "ESSENTIAL"}]</t>
-  </si>
-  <si>
     <t>What is the subsystem for the engine?</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>What is the effect of leaks on the transmission hydraulics?</t>
-  </si>
-  <si>
-    <t>Name matching, Semantic matching</t>
   </si>
   <si>
     <t>Which subcomponent of Power unit has an RPN of 27.</t>
@@ -8547,9 +8541,6 @@
     <t>[{"nugget": "The failure mode with the highest detection value in the Power Train is Wearing.", "status": "ESSENTIAL"}, {"nugget": "The Wearing failure mode has a detection value of 5.", "status": "ESSENTIAL"}, {"nugget": "The Wearing failure mode occurs in the Axles component and Differential subcomponent.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
-    <t>[{"nugget": "Multiple failure modes are associated with leaks in the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "The failure mode with the highest occurrence value is 'Leaks'.", "status": "ESSENTIAL"}, {"nugget": "'Leaks' occurs in the Cooling System component of the Power Unit subsystem.", "status": "ESSENTIAL"}, {"nugget": "'Leaks' occurs in the Radiator subcomponent of the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "The occurrence value for 'Leaks' is 4.", "status": "ESSENTIAL"}]</t>
-  </si>
-  <si>
     <t>[{"nugget": "The component with the highest number of failures is the Data Collection Unit (DCU).", "status": "ESSENTIAL"}, {"nugget": "The DCU is part of the Electrical System subsystem.", "status": "OPTIONAL"}, {"nugget": "The DCU has 41 failure modes.", "status": "ESSENTIAL"}, {"nugget": "All failure modes of the DCU have a severity of 2, there is not a single most severe failure mode.", "status": "ESSENTIAL"}]</t>
   </si>
   <si>
@@ -8565,9 +8556,6 @@
     <t>[{"nugget": "The Leaking failure mode in the Suspension Cylinder subcomponent has the failure cause 'General wear and tear, Physical impacts, incorrect installation of seals'.", "status": "ESSENTIAL"}, {"nugget": "The Wearing failure mode in the Suspension Bushing subcomponent has the failure cause 'Wearing over time'.", "status": "ESSENTIAL"}, {"nugget": "The Leaking failure mode in the Steering Cylinder subcomponent has the failure cause 'General wear and tear, physical impacts, incorrect installation of seal or cylinder'.", "status": "ESSENTIAL"}, {"nugget": "The Leaking failure mode in the Hoist Cylinder subcomponent has the failure cause 'General wear and tear, physical impacts, incorrect installation of seal or cylinder'.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant failure modes.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
-    <t>[{"nugget": "The subcomponent Fuses of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Fuses is on the Electrical System subcomponent.", "status": "OPTIONAL"}, {"nugget": "The subcomponent Wiring Harness of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Wiring Harness is on the Electrical System subcomponent.", "status": "OPTIONAL"}, {"nugget": "The subcomponent Turbocharger of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Turbocharger is on the Air Intake System subcomponent.", "status": "OPTIONAL"}, {"nugget": "There are no other relevant subcomponents.", "status": "OPTIONAL"}]</t>
-  </si>
-  <si>
     <t>[{"nugget": "The failure cause of Overloading in ECU in the power train is 'Shorting of sensor power surge'.", "status": "ESSENTIAL"}, {"nugget": "ECU refers to the Electronic Control Unit (ECU) subcomponent.", "status": "OPTIONAL"}, {"nugget": "There are no other relevant failure modes.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
@@ -8580,9 +8568,6 @@
     <t>[{"nugget": "The failure mode Corrosion in the Batteries subcomponent has an RPN of 18.", "status": "ESSENTIAL"}, {"nugget": "The failure mode Wearing in the Batteries subcomponent has an RPN of 8.", "status": "ESSENTIAL"}, {"nugget": "The failure mode End of usable life in the Batteris subcomponent has an RPN of 12.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant failure modes.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
-    <t>[{"nugget": "The Transmission component has 3 failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Transmission's relevant failure modes are Wearing in Electronic Control Unit (ECU), Corrosion in the Electronic Control Unit (ECU), and Wearing in the Planetary Gear Sets, all with RPNs of 36", "status": "ESSENTIAL"}, {"nugget": "The Upbox component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Upbox's relevant failure mode is Wearing in the Gears with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "The Dropbox component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Dropbox's relevant failure mode is Wearing in the Gears with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "The Cooling System component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Cooling System's relevant failure mode is Mechanical Failure in the Water Pump with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant components and failure modes.", "status": "OPTIONAL"}]</t>
-  </si>
-  <si>
     <t>[{"nugget": "The Fuel System component in the Power Unit subsystem has a failure mode named Blocked.", "status": "ESSENTIAL"}, {"nugget": "The Fuel System's relevant failure mode is in the Fuel Filter subcomponent.", "status": "OPTIONAL"}, {"nugget": "The Lubrication System component in the Power Unit subsystem has failure modes named Blocked.", "status": "ESSENTIAL"}, {"nugget": "The Lubrication System's 3 relevant failure modes is in the Oil Cooler, Oil Filter and Lubrication lines subcomponents.", "status": "OPTIONAL"},  {"nugget": "The Air-conditioning component in the Electrical System subsystem has a failure mode named Blocked.", "status": "ESSENTIAL"}, {"nugget": "The Air-conditioning's relevant failure mode is in the Filter subcomponent.", "status": "OPTIONAL"}, {"nugget": "There are no other relevant failure modes, components and subsystems.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
@@ -8604,15 +8589,9 @@
     <t>[{"nugget": "The Fuel System has a failure mode where the recommended action is 'Drain and flush the fuel tank during 1000 hour service'.", "status": "ESSENTIAL"}, {"nugget": "This action addresses the 'Cracked and Leaking' failure mode on the Fuel Tank subcomponent.", "status": "ESSENTIAL"}, {"nugget": "All other recommended actions in the Fuel System simply prescibe checks and inspections.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
-    <t>[{"nugget": "Corrosion on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) component, has the failure effect 'Reduced ability to successfully move machinery safely' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) component, has the failure effect 'Reduced ability to successfully move machinery safely' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Hand Rails subcomponent of the Power Frame subsystem and Hoods and Covers component, has the failure effect 'Difficulty in gaining access to machine above safe working height' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cabin Assembly subcomponent of the Power Frame subsystem and Cabin component, has the failure effect 'Unsafe working environment, windows, and doors no longer fit' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Drivers Seat subcomponent of the Power Frame subsystem and Cabin component, has the failure effect 'Unsafe working environment, windows, and doors no longer fit' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Drivers Seat subcomponent of the Power Frame subsystem and Cabin component, has the failure cause 'Unsafe working environment' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Overloading on the Grease Pump subcomponent of the Power Frame subsystem and Greasing system component, has the failure effect 'Shorting of live wires to ground, or electrical component failure' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "There are also other failure modes below severity score of 3 that may indirectly affect personnel safety, such as fire hazards and false readings.", "status": "OPTIONAL"}]</t>
-  </si>
-  <si>
     <t>[{"nugget": "The Physical Damage failure mode on the Air filter housing subcomponent has the current control 'Visual inspection daily for damages'.", "status": "ESSENTIAL"}, {"nugget": "The Leaking failure mode on the Turbocharger subcomponent has the current control 'Inspect induction hoses and joints every 125 hour service'.", "status": "ESSENTIAL"}, {"nugget": "The Physical damage failure mode on the Charge Air Cooler subcomponent has the current control 'Visual inspection on 125 hour services'.", "status": "ESSENTIAL"}, {"nugget": "The Physical damage failure mode on the Inlet Manifold subcomponent has the current control 'Visual inspection on 125 hour services'.", "status": "ESSENTIAL"}, {"nugget": "The Leaking failure mode on the Inlet Manifold subcomponent has the current control 'Visual inspection on 125 hour services'.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant failure modes and current controls.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
-    <t>[{"nugget": "Corrosion in the Transmission component and Electronic Control Unit (ECU) subcomponent has the recommended action 'Investigate method to include auto-electrical servicing in PM services. Grease (add sealant) all connections and plugs every 500 hour service'.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Drivelines component and Articulation Driveline subcomponent has the recommended action 'Inspect and lubricate driveline slip joint and universal joints on 125\ hour service. Inspect for optimal replacement interval of component'.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant failure modes and recommended actions.", "status": "OPTIONAL"}]</t>
-  </si>
-  <si>
     <t>[{"nugget": "Cracked or leaking in the Fuel Tank subcomponent has the failure effect 'Fuel loss, fire'.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Cooler subcomponent has the failure effect 'Loss of power, engine overheating'.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Fuel Cooler subcomponent has the failure effect 'Loss of power, engine overheating'.", "status": "ESSENTIAL"}, {"nugget": "Mechanical failure in the Fuel Cooler subcomponent has the failure effect 'Fuel overheating'.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Filter subcomponent has the failure effect 'Loss of power, fire'.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Fuel Filter subcomponent has the failure effect 'Fuel leak, fire'.", "status": "ESSENTIAL"}, {"nugget": "Leaking in the Fuel Lines/Rail subcomponent has the failure effect 'Loss of power, fire'.", "status": "ESSENTIAL"}, {"nugget": "Physical damage in the Fuel Lines/Rail subcomponent has the failure effect 'Loss of power, fire'.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant failure modes.", "status": "OPTIONAL"}]</t>
   </si>
   <si>
@@ -8626,13 +8605,31 @@
   </si>
   <si>
     <t>[{"nugget": "The Air Intake System has a failure mode with a recommended action called 'Reaches end of usable life'.", "status": "ESSENTIAL"}, {"nugget": "This failure mode occurs in the air filter subcomponent.", "status": "OPTIONAL"}, {"nugget": "The recommended action is 'Check air filter indicators during daily inspections'", "status": "ESSENTIAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "The subcomponent Fuses of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Fuses is on the Electrical System component.", "status": "OPTIONAL"}, {"nugget": "The subcomponent Wiring Harness of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Wiring Harness is on the Electrical System component.", "status": "OPTIONAL"}, {"nugget": "The subcomponent Turbocharger of the Power Unit has an RPN of 27.", "status": "ESSENTIAL"}, {"nugget": "The relevant subcomponent Turbocharger is on the Air Intake System component.", "status": "OPTIONAL"}, {"nugget": "There are no other relevant subcomponents.", "status": "OPTIONAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "The Transmission component has failure modes with RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Transmission's relevant failure modes are Wearing in Electronic Control Unit (ECU), Corrosion in the Electronic Control Unit (ECU), and Wearing in the Planetary Gear Sets, all with RPNs of 36", "status": "ESSENTIAL"}, {"nugget": "The Upbox component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Upbox's relevant failure mode is Wearing in the Gears with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "The Dropbox component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Dropbox's relevant failure mode is Wearing in the Gears with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "The Cooling System component has a failure mode with an RPN over 35.", "status": "ESSENTIAL"}, {"nugget": "The Cooling System's relevant failure mode is Mechanical Failure in the Water Pump with an RPN of 36.", "status": "ESSENTIAL"}, {"nugget": "There are no other relevant components and failure modes.", "status": "OPTIONAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "Multiple failure modes are associated with leaks in the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "The failure mode with the highest occurrence value is 'Leaks'.", "status": "ESSENTIAL"}, {"nugget": "'Leaks' occurs in the Cooling System component of the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "'Leaks' occurs in the Radiator subcomponent of the Power Unit subsystem.", "status": "OPTIONAL"}, {"nugget": "The occurrence value for 'Leaks' is 4.", "status": "ESSENTIAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "Corrosion on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) component, has the failure effect 'Reduced ability to successfully move machinery safely' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cameras subcomponent of the Electrical System subsystem and Data Collection Unit (DCU) component, has the failure effect 'Reduced ability to successfully move machinery safely' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Hand Rails subcomponent of the Power Frame subsystem and Hoods and Covers component, has the failure effect 'Difficulty in gaining access to machine above safe working height' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Cabin Assembly subcomponent of the Power Frame subsystem and Cabin component, has the failure effect 'Unsafe working environment, windows, and doors no longer fit' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Drivers Seat subcomponent of the Power Frame subsystem and Cabin component, has the failure effect 'Unsafe working environment, windows, and doors no longer fit' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Wearing on the Windows subcomponent of the Power Frame subsystem and Cabin component, has the failure cause 'Unsafe working environment' and severity of 2.", "status": "ESSENTIAL"}, {"nugget": "Overloading on the Grease Pump subcomponent of the Power Frame subsystem and Greasing system component, has the failure effect 'Shorting of live wires to ground, or electrical component failure' and severity of 2.", "status": "OPTIONAL"}, {"nugget": "There are also other failure modes below severity score of 3 that may indirectly affect personnel safety, such as fire hazards and false readings.", "status": "OPTIONAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "The condenser has a failure mode called Leaking.", "status": "ESSENTIAL"}, {"nugget": "The RPN for the condenser leaking failure mode is 18.", "status": "ESSENTIAL"}]</t>
+  </si>
+  <si>
+    <t>[{"nugget": "Corrosion in the Transmission component and Electronic Control Unit (ECU) subcomponent has the recommended action 'Investigate method to include auto-electrical servicing in PM services. Grease (add sealant) all connections and plugs every 500 hour service'.", "status": "ESSENTIAL"}, {"nugget": "Wearing in the Drivelines component and Articulation Driveline subcomponent has the recommended action 'Inspect and lubricate driveline slip joint and universal joints on 125\ hour service. Inspect for optimal replacement interval of component'.", "status": "ESSENTIAL"}, {"nugget": "Some recommended actions related to oil samples can be considered relevant, but aside from this there are no other stated failure modes and recommended actions.", "status": "OPTIONAL"}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8645,13 +8642,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -8697,7 +8687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -8708,16 +8698,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9024,15 +9008,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="48.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="1"/>
@@ -9045,7 +9029,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -9062,14 +9046,14 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>72</v>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9077,16 +9061,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9094,16 +9078,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>74</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9111,16 +9095,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>75</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
@@ -9128,16 +9112,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -9145,16 +9129,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -9162,16 +9146,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>78</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="160" x14ac:dyDescent="0.2">
@@ -9179,16 +9163,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="240" x14ac:dyDescent="0.2">
@@ -9196,16 +9180,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
+        <v>108</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -9213,16 +9197,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>81</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="335" x14ac:dyDescent="0.2">
@@ -9230,16 +9214,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>82</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9247,16 +9231,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="256" x14ac:dyDescent="0.2">
@@ -9264,16 +9248,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>83</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -9281,16 +9265,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>84</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -9298,16 +9282,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>85</v>
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9315,16 +9299,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9332,16 +9316,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9349,16 +9333,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="288" x14ac:dyDescent="0.2">
@@ -9366,16 +9350,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>89</v>
+        <v>38</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -9383,16 +9367,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>90</v>
+        <v>40</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="208" x14ac:dyDescent="0.2">
@@ -9400,16 +9384,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>91</v>
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9417,16 +9401,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>92</v>
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9434,16 +9418,16 @@
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9451,16 +9435,16 @@
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>94</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -9468,16 +9452,16 @@
         <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>95</v>
+        <v>49</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9485,16 +9469,16 @@
         <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>96</v>
+        <v>50</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -9502,16 +9486,16 @@
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>97</v>
+        <v>51</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="256" x14ac:dyDescent="0.2">
@@ -9519,16 +9503,16 @@
         <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>98</v>
+        <v>52</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="320" x14ac:dyDescent="0.2">
@@ -9536,16 +9520,16 @@
         <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>99</v>
+        <v>53</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9553,16 +9537,16 @@
         <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>100</v>
+        <v>54</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -9570,16 +9554,16 @@
         <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>101</v>
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="304" x14ac:dyDescent="0.2">
@@ -9587,16 +9571,16 @@
         <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>102</v>
+        <v>58</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -9604,16 +9588,16 @@
         <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>103</v>
+        <v>59</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="288" x14ac:dyDescent="0.2">
@@ -9621,16 +9605,16 @@
         <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>104</v>
+        <v>61</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -9638,16 +9622,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>105</v>
+        <v>62</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="407" customHeight="1" x14ac:dyDescent="0.2">
@@ -9655,16 +9639,16 @@
         <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>106</v>
+        <v>63</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -9672,16 +9656,16 @@
         <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>107</v>
+        <v>64</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="320" x14ac:dyDescent="0.2">
@@ -9689,16 +9673,16 @@
         <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -9706,16 +9690,16 @@
         <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>108</v>
+        <v>66</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -9723,16 +9707,16 @@
         <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>